<commit_message>
1st commit on QA Branch discussion needed
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/Automation_Sample.xlsx
+++ b/src/main/resources/TestData/Automation_Sample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24722"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8706CBF-F77E-41C4-96D0-B07F858AA6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACBEF458-530E-438E-AC48-5A19A840F274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,12 +26,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
   <si>
     <t>anu.bhat@harbingergroup.com</t>
   </si>
   <si>
     <t>Data_123</t>
+  </si>
+  <si>
+    <t>Anu</t>
+  </si>
+  <si>
+    <t>Bhat</t>
+  </si>
+  <si>
+    <t>Super User</t>
   </si>
 </sst>
 </file>
@@ -394,28 +418,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{F5DB54E3-C020-42E9-AB03-9330F4FA3EB5}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F5DB54E3-C020-42E9-AB03-9330F4FA3EB5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>